<commit_message>
Chore: Diagramas de Casos de Uso, Classes, ER, Domínio
</commit_message>
<xml_diff>
--- a/documentação/UC_RF_RNF.xlsx
+++ b/documentação/UC_RF_RNF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://criticalmfg-my.sharepoint.com/personal/eduardooliveira_criticalmanufacturing_com/Documents/Personal/UMinhoMEI/ano_1/a1_semestre_2/_aa/trabalho_prático/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\ea-project\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_AD4D361C20488DEA4E38A0A22C1C69C45BDEDD85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{566055A3-E806-4FBE-B3A6-398D15CA447C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2887CF8D-5F43-40F7-9B30-36628829F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos Funcionais" sheetId="6" r:id="rId1"/>
@@ -18,14 +18,25 @@
     <sheet name="Casos de Uso" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="2" hidden="1">'Casos de Uso'!$A$1:$F$16</definedName>
+    <definedName name="DadosExternos_1" localSheetId="2" hidden="1">'Casos de Uso'!$A$1:$F$11</definedName>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'Requisitos Funcionais'!$A$1:$H$15</definedName>
     <definedName name="DadosExternos_1" localSheetId="1" hidden="1">'Requisitos Não Funcionais'!$A$1:$G$11</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="173">
   <si>
     <t>Use Case</t>
   </si>
@@ -69,9 +80,6 @@
     <t>Sistema</t>
   </si>
   <si>
-    <t>O sistema está disponível para configuração da competição.</t>
-  </si>
-  <si>
     <t>As configurações da competição são salvas no sistema.</t>
   </si>
   <si>
@@ -81,21 +89,9 @@
     <t>As provas são criadas e Registadas no sistema.</t>
   </si>
   <si>
-    <t>O sistema está disponível para criar uma competição.</t>
-  </si>
-  <si>
-    <t>A competição é criada e Registada no sistema.</t>
-  </si>
-  <si>
     <t>Inserção de Resultados</t>
   </si>
   <si>
-    <t>O sistema está disponível para inserir resultados de competição.</t>
-  </si>
-  <si>
-    <t>Os resultados da competição são registados no sistema.</t>
-  </si>
-  <si>
     <t>Publicação de Resultados</t>
   </si>
   <si>
@@ -138,21 +134,12 @@
     <t>Os escalões são registados no sistema.</t>
   </si>
   <si>
-    <t>O sistema está disponível para definir categorias de competição.</t>
-  </si>
-  <si>
     <t>As notificações são enviadas por email para os destinatários.</t>
   </si>
   <si>
     <t>Protesto de Resultado</t>
   </si>
   <si>
-    <t>Os resultados da competição estão disponíveis para consulta.</t>
-  </si>
-  <si>
-    <t>O protesto é registado no sistema e enviado ao organizador da competição.</t>
-  </si>
-  <si>
     <t>Administrador</t>
   </si>
   <si>
@@ -174,9 +161,6 @@
     <t>As informações meteorológicas são registadas no sistema.</t>
   </si>
   <si>
-    <t>As categorias são registadas no sistema.</t>
-  </si>
-  <si>
     <t>Equipa</t>
   </si>
   <si>
@@ -192,9 +176,6 @@
     <t>Inserção e Atualização da Meteorologia</t>
   </si>
   <si>
-    <t>Introduzir Horário de Provas e Competições</t>
-  </si>
-  <si>
     <t>Definição das Categorias de Provas e Competições</t>
   </si>
   <si>
@@ -354,9 +335,6 @@
     <t>O sistema deve permitir aos organizadores inserir horários de provas e competições no sistema</t>
   </si>
   <si>
-    <t>Os horários das provas são registrados no sistema.</t>
-  </si>
-  <si>
     <t>RF10</t>
   </si>
   <si>
@@ -546,17 +524,74 @@
     <t>O sistema deve permitir enviar notificações de eventos aos respetivos destinatários</t>
   </si>
   <si>
-    <t>Notificação de Eventos</t>
+    <t>Prioridade (MoSCoW)</t>
+  </si>
+  <si>
+    <t>Would</t>
+  </si>
+  <si>
+    <t>Gestão de Provas e Competições</t>
+  </si>
+  <si>
+    <t>Os as provas e respetivos horários das provas são registrados no sistema.</t>
+  </si>
+  <si>
+    <t>Could</t>
+  </si>
+  <si>
+    <t>Gerir Atletas</t>
+  </si>
+  <si>
+    <t>Gerir Equipas</t>
+  </si>
+  <si>
+    <t>Gerir Clubes</t>
+  </si>
+  <si>
+    <t>Gerir Competições</t>
+  </si>
+  <si>
+    <t>Gerir Organizadores</t>
+  </si>
+  <si>
+    <t>Gerir Prova</t>
+  </si>
+  <si>
+    <t>Gerir Resultados</t>
+  </si>
+  <si>
+    <t>Gerir Escalões</t>
+  </si>
+  <si>
+    <t>Gerir Informação Meteorológica</t>
+  </si>
+  <si>
+    <t>Gerir Eventos</t>
+  </si>
+  <si>
+    <t>Cenário Normal</t>
+  </si>
+  <si>
+    <t>Alternativa 1</t>
+  </si>
+  <si>
+    <t>Alternativa N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -582,13 +617,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -700,14 +745,17 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_1" connectionId="1" xr16:uid="{9DEA9C5D-C6D1-42F5-B285-8D651E1C1D37}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7">
-    <queryTableFields count="6">
+  <queryTableRefresh nextId="11" unboundColumnsRight="3">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Use Case" tableColumnId="1"/>
       <queryTableField id="2" name="Nome" tableColumnId="2"/>
       <queryTableField id="3" name="Ator Principal" tableColumnId="3"/>
       <queryTableField id="4" name="Atores secundários" tableColumnId="4"/>
       <queryTableField id="5" name="Pré-Condições" tableColumnId="5"/>
       <queryTableField id="6" name="Pós-Condições" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="8"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="10"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="9"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -717,14 +765,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{44FB398C-29E9-4A26-A46C-32A737AAA707}" name="Requisitos_Funcionais" displayName="Requisitos_Funcionais" ref="A1:H15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H15" xr:uid="{44FB398C-29E9-4A26-A46C-32A737AAA707}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F09E7A9-8298-4F77-95F6-94BF234683CA}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B6196257-4C6D-4AFA-B520-16654ABEC03E}" uniqueName="2" name="Tipo de Requisito" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{0D0A4628-8EDB-40CF-A35A-8D110A8122E8}" uniqueName="3" name="Use Cases" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{78BD77F0-F5D2-48B3-8792-C0781C159F90}" uniqueName="4" name="Nome do Requisito" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{2A2B6552-EB11-4D6E-BA5B-CC98B3F29B93}" uniqueName="5" name="Descrição" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{F4A73330-5AF9-40CA-9C87-547629D02B18}" uniqueName="6" name="Origem do requisito" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{6C5288F0-65AC-45D5-9CD8-0E78419F6B99}" uniqueName="7" name="Fit Criterion" queryTableFieldId="7" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{B1027064-B122-4B7A-A19E-A66469326436}" uniqueName="8" name="Prioridade" queryTableFieldId="8" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{5F09E7A9-8298-4F77-95F6-94BF234683CA}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B6196257-4C6D-4AFA-B520-16654ABEC03E}" uniqueName="2" name="Tipo de Requisito" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{0D0A4628-8EDB-40CF-A35A-8D110A8122E8}" uniqueName="3" name="Use Cases" queryTableFieldId="3" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{78BD77F0-F5D2-48B3-8792-C0781C159F90}" uniqueName="4" name="Nome do Requisito" queryTableFieldId="4" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{2A2B6552-EB11-4D6E-BA5B-CC98B3F29B93}" uniqueName="5" name="Descrição" queryTableFieldId="5" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{F4A73330-5AF9-40CA-9C87-547629D02B18}" uniqueName="6" name="Origem do requisito" queryTableFieldId="6" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{6C5288F0-65AC-45D5-9CD8-0E78419F6B99}" uniqueName="7" name="Fit Criterion" queryTableFieldId="7" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{B1027064-B122-4B7A-A19E-A66469326436}" uniqueName="8" name="Prioridade (MoSCoW)" queryTableFieldId="8" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,28 +782,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96549181-928E-4782-A5C9-0FAAD3A833EF}" name="Requisitos_Não_Funcionais" displayName="Requisitos_Não_Funcionais" ref="A1:G11" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G11" xr:uid="{96549181-928E-4782-A5C9-0FAAD3A833EF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{47E10CFE-606E-41C1-8EE4-8F13D4830CFE}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{9780A8FF-FBF4-4217-B2A6-76069B76DEF5}" uniqueName="2" name="Nome do Requisito" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F01A3D5B-473B-4AEF-8D79-4D8B9979B05D}" uniqueName="3" name="Tipo de Requisito" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{526DCAAC-FE24-4303-919B-45AA50B9FE1F}" uniqueName="4" name="Descrição" queryTableFieldId="4" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{4887D9D6-9077-4626-8F17-8A73BE3343EA}" uniqueName="5" name="Origem do requisito" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{5ADCAB05-C5B4-49F3-8B2D-9F224E312F97}" uniqueName="6" name="Fit Criterion" queryTableFieldId="6" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{E6472B2E-99D4-447D-8AEE-16086B22ABE3}" uniqueName="7" name="Prioridade" queryTableFieldId="7" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{47E10CFE-606E-41C1-8EE4-8F13D4830CFE}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{9780A8FF-FBF4-4217-B2A6-76069B76DEF5}" uniqueName="2" name="Nome do Requisito" queryTableFieldId="2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F01A3D5B-473B-4AEF-8D79-4D8B9979B05D}" uniqueName="3" name="Tipo de Requisito" queryTableFieldId="3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{526DCAAC-FE24-4303-919B-45AA50B9FE1F}" uniqueName="4" name="Descrição" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4887D9D6-9077-4626-8F17-8A73BE3343EA}" uniqueName="5" name="Origem do requisito" queryTableFieldId="5" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{5ADCAB05-C5B4-49F3-8B2D-9F224E312F97}" uniqueName="6" name="Fit Criterion" queryTableFieldId="6" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{E6472B2E-99D4-447D-8AEE-16086B22ABE3}" uniqueName="7" name="Prioridade" queryTableFieldId="7" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A7DC22B7-D72A-4807-B002-0C2BC540A232}" name="Casos_de_Uso" displayName="Casos_de_Uso" ref="A1:F16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F16" xr:uid="{A7DC22B7-D72A-4807-B002-0C2BC540A232}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C890EB42-E96D-4855-B6B0-76902B1DBBCD}" uniqueName="1" name="Use Case" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{45B1453F-FEBC-4CBD-808A-02428A686DCE}" uniqueName="2" name="Nome" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D2642693-3DF6-4D3B-9AEA-23A35433057F}" uniqueName="3" name="Ator Principal" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6DA39132-9E24-44C4-BD28-E759EA7B2790}" uniqueName="4" name="Atores secundários" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{5A34DC70-016B-46F7-9354-C940C4569F5A}" uniqueName="5" name="Pré-Condições" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{07051044-7847-49CB-A313-848B3238593E}" uniqueName="6" name="Pós-Condições" queryTableFieldId="6" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A7DC22B7-D72A-4807-B002-0C2BC540A232}" name="Casos_de_Uso" displayName="Casos_de_Uso" ref="A1:I11" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I11" xr:uid="{A7DC22B7-D72A-4807-B002-0C2BC540A232}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{C890EB42-E96D-4855-B6B0-76902B1DBBCD}" uniqueName="1" name="Use Case" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{45B1453F-FEBC-4CBD-808A-02428A686DCE}" uniqueName="2" name="Nome" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D2642693-3DF6-4D3B-9AEA-23A35433057F}" uniqueName="3" name="Ator Principal" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{6DA39132-9E24-44C4-BD28-E759EA7B2790}" uniqueName="4" name="Atores secundários" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{5A34DC70-016B-46F7-9354-C940C4569F5A}" uniqueName="5" name="Pré-Condições" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{07051044-7847-49CB-A313-848B3238593E}" uniqueName="6" name="Pós-Condições" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{29DD4656-69D9-4582-9FC7-79CC87D13C6A}" uniqueName="8" name="Cenário Normal" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{73558F76-05ED-4B50-ACAE-F368228DCE62}" uniqueName="10" name="Alternativa 1" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{751A5E1A-031B-4D29-9541-FC5CE20003E7}" uniqueName="9" name="Alternativa N" queryTableFieldId="8" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1026,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD8EB55-FF9F-4F31-AE8A-93474497F49D}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,397 +1090,397 @@
     <col min="5" max="5" width="95" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="H15" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1496,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,261 +1506,261 @@
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="158.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="147.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="103.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" t="s">
         <v>122</v>
       </c>
-      <c r="D4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" t="s">
-        <v>133</v>
-      </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G8" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G9" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F10" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G11" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1722,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FEBA9D-0188-495E-B043-96CC097CC564}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,9 +1787,12 @@
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="87.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1757,116 +1811,140 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -1875,190 +1953,106 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>